<commit_message>
add fuction getDEmand of this service
</commit_message>
<xml_diff>
--- a/Service_plan_form/demand_format/demandTFtestXLSX_new.xlsx
+++ b/Service_plan_form/demand_format/demandTFtestXLSX_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATCHAPCYP\Downloads\demand_format\demand_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C90CAD-4EEE-46C2-B3FB-21AAA5DD6959}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DFCC5A-D663-4AE4-847C-060FD6885966}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{D39FB900-15C1-7B47-8F01-B0CA86C94EDD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="4" xr2:uid="{D39FB900-15C1-7B47-8F01-B0CA86C94EDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Station1" sheetId="1" r:id="rId1"/>
@@ -104,17 +104,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -447,16 +437,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783E6E19-8982-3D4E-8148-6314C244FA37}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -479,12 +469,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" s="3">
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="3">
-        <v>0.375</v>
+        <v>0.3756944444444445</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -502,7 +492,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" s="3">
         <v>0.375</v>
       </c>
@@ -525,7 +515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" s="3">
         <v>0.41666666666666669</v>
       </c>
@@ -548,7 +538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" s="3">
         <v>0.45833333333333331</v>
       </c>
@@ -571,7 +561,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" s="3">
         <v>0.5</v>
       </c>
@@ -594,7 +584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" s="3">
         <v>0.54166666666666663</v>
       </c>
@@ -617,7 +607,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" s="3">
         <v>0.58333333333333304</v>
       </c>
@@ -640,7 +630,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" s="3">
         <v>0.625</v>
       </c>
@@ -663,7 +653,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" s="3">
         <v>0.66666666666666696</v>
       </c>
@@ -686,7 +676,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" s="3">
         <v>0.70833333333333304</v>
       </c>
@@ -711,7 +701,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:B11">
-    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="lastWeek">
+    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(A2,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(A2,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -724,15 +714,15 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:G11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -755,12 +745,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="3">
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="3">
-        <v>0.375</v>
+        <v>0.3756944444444445</v>
       </c>
       <c r="C2" s="2">
         <v>212</v>
@@ -778,7 +768,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" s="3">
         <v>0.375</v>
       </c>
@@ -801,7 +791,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" s="3">
         <v>0.41666666666666669</v>
       </c>
@@ -824,7 +814,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" s="3">
         <v>0.45833333333333331</v>
       </c>
@@ -847,7 +837,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" s="3">
         <v>0.5</v>
       </c>
@@ -870,7 +860,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7" s="3">
         <v>0.54166666666666663</v>
       </c>
@@ -893,7 +883,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A8" s="3">
         <v>0.58333333333333304</v>
       </c>
@@ -917,7 +907,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9" s="3">
         <v>0.625</v>
       </c>
@@ -941,7 +931,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A10" s="3">
         <v>0.66666666666666696</v>
       </c>
@@ -965,7 +955,7 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A11" s="3">
         <v>0.70833333333333304</v>
       </c>
@@ -999,15 +989,15 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="C8:D12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1030,12 +1020,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="1">
-        <v>0.375</v>
+        <v>0.38194444444444442</v>
       </c>
       <c r="C2">
         <v>313</v>
@@ -1053,12 +1043,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>0.375</v>
       </c>
       <c r="B3" s="1">
-        <v>0.41666666666666702</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="C3">
         <v>31</v>
@@ -1076,7 +1066,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>0.41666666666666702</v>
       </c>
@@ -1099,7 +1089,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>0.45833333333333298</v>
       </c>
@@ -1122,7 +1112,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>0.5</v>
       </c>
@@ -1145,7 +1135,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>0.54166666666666696</v>
       </c>
@@ -1168,7 +1158,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>0.58333333333333404</v>
       </c>
@@ -1191,7 +1181,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>0.625000000000001</v>
       </c>
@@ -1214,7 +1204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>0.66666666666666796</v>
       </c>
@@ -1237,7 +1227,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>0.70833333333333504</v>
       </c>
@@ -1270,15 +1260,15 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1301,12 +1291,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="1">
-        <v>0.375</v>
+        <v>0.3756944444444445</v>
       </c>
       <c r="C2">
         <v>414</v>
@@ -1324,12 +1314,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>0.375</v>
       </c>
       <c r="B3" s="1">
-        <v>0.41666666666666702</v>
+        <v>0.41736111111111113</v>
       </c>
       <c r="C3">
         <v>41</v>
@@ -1347,7 +1337,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>0.41666666666666702</v>
       </c>
@@ -1370,7 +1360,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>0.45833333333333298</v>
       </c>
@@ -1393,7 +1383,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>0.5</v>
       </c>
@@ -1416,7 +1406,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>0.54166666666666696</v>
       </c>
@@ -1439,7 +1429,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>0.58333333333333404</v>
       </c>
@@ -1463,7 +1453,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>0.625000000000001</v>
       </c>
@@ -1487,7 +1477,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>0.66666666666666796</v>
       </c>
@@ -1511,7 +1501,7 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>0.70833333333333504</v>
       </c>
@@ -1544,16 +1534,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1338C68A-BFB5-4B6E-84B8-51079048C625}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1576,7 +1566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" s="3">
         <v>0.33333333333333331</v>
       </c>
@@ -1599,12 +1589,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" s="3">
         <v>0.375</v>
       </c>
       <c r="B3" s="3">
-        <v>0.41666666666666669</v>
+        <v>0.41736111111111113</v>
       </c>
       <c r="C3">
         <v>51</v>
@@ -1622,12 +1612,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" s="3">
         <v>0.41666666666666669</v>
       </c>
       <c r="B4" s="3">
-        <v>0.45833333333333331</v>
+        <v>0.45902777777777781</v>
       </c>
       <c r="C4">
         <v>515</v>
@@ -1645,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" s="3">
         <v>0.45833333333333331</v>
       </c>
@@ -1668,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" s="3">
         <v>0.5</v>
       </c>
@@ -1691,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" s="3">
         <v>0.54166666666666663</v>
       </c>
@@ -1714,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" s="3">
         <v>0.58333333333333304</v>
       </c>
@@ -1737,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" s="3">
         <v>0.625</v>
       </c>
@@ -1760,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" s="3">
         <v>0.66666666666666696</v>
       </c>
@@ -1783,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" s="3">
         <v>0.70833333333333304</v>
       </c>
@@ -1808,7 +1798,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:B11">
-    <cfRule type="timePeriod" dxfId="2" priority="1" timePeriod="lastWeek">
+    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(A2,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(A2,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
calculate by carry demand for all service
</commit_message>
<xml_diff>
--- a/Service_plan_form/demand_format/demandTFtestXLSX_new.xlsx
+++ b/Service_plan_form/demand_format/demandTFtestXLSX_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATCHAPCYP\Downloads\demand_format\demand_format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATCHAPCYP\Repository\Service_plan_form\Service_plan_form\demand_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DFCC5A-D663-4AE4-847C-060FD6885966}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B094F2-700A-4A30-BE54-07B098FF502A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="4" xr2:uid="{D39FB900-15C1-7B47-8F01-B0CA86C94EDD}"/>
+    <workbookView xWindow="4372" yWindow="923" windowWidth="14400" windowHeight="8272" activeTab="4" xr2:uid="{D39FB900-15C1-7B47-8F01-B0CA86C94EDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Station1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -480,16 +480,16 @@
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>12</v>
+        <v>182</v>
       </c>
       <c r="E2" s="2">
-        <v>13</v>
+        <v>183</v>
       </c>
       <c r="F2" s="2">
-        <v>14</v>
+        <v>184</v>
       </c>
       <c r="G2" s="2">
-        <v>15</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.5">
@@ -503,16 +503,16 @@
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>121</v>
+        <v>192</v>
       </c>
       <c r="E3" s="2">
-        <v>13</v>
+        <v>193</v>
       </c>
       <c r="F3" s="2">
-        <v>14</v>
+        <v>194</v>
       </c>
       <c r="G3" s="2">
-        <v>15</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
@@ -526,16 +526,16 @@
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="E4" s="2">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="F4" s="2">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="G4" s="2">
-        <v>15</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
@@ -549,16 +549,16 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="E5" s="2">
-        <v>13</v>
+        <v>113</v>
       </c>
       <c r="F5" s="2">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="G5" s="2">
-        <v>15</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
@@ -572,16 +572,16 @@
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>12</v>
+        <v>122</v>
       </c>
       <c r="E6" s="2">
-        <v>13</v>
+        <v>123</v>
       </c>
       <c r="F6" s="2">
-        <v>14</v>
+        <v>124</v>
       </c>
       <c r="G6" s="2">
-        <v>15</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
@@ -595,16 +595,16 @@
         <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="E7" s="2">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="F7" s="2">
-        <v>14</v>
+        <v>134</v>
       </c>
       <c r="G7" s="2">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.5">
@@ -618,16 +618,16 @@
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="E8" s="2">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="F8" s="2">
-        <v>14</v>
+        <v>144</v>
       </c>
       <c r="G8" s="2">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.5">
@@ -641,16 +641,16 @@
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E9" s="2">
-        <v>13</v>
+        <v>153</v>
       </c>
       <c r="F9" s="2">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="G9" s="2">
-        <v>411</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.5">
@@ -664,16 +664,16 @@
         <v>0</v>
       </c>
       <c r="D10" s="2">
-        <v>121</v>
+        <v>162</v>
       </c>
       <c r="E10" s="2">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="F10" s="2">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="G10" s="2">
-        <v>242</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
@@ -687,16 +687,16 @@
         <v>0</v>
       </c>
       <c r="D11" s="2">
-        <v>121</v>
+        <v>172</v>
       </c>
       <c r="E11" s="2">
-        <v>13</v>
+        <v>173</v>
       </c>
       <c r="F11" s="2">
-        <v>142</v>
+        <v>174</v>
       </c>
       <c r="G11" s="2">
-        <v>242</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -714,7 +714,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F2" sqref="F2:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -753,19 +753,19 @@
         <v>0.3756944444444445</v>
       </c>
       <c r="C2" s="2">
-        <v>212</v>
+        <v>281</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>23</v>
+        <v>283</v>
       </c>
       <c r="F2" s="2">
-        <v>24</v>
+        <v>284</v>
       </c>
       <c r="G2" s="2">
-        <v>25</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.5">
@@ -776,19 +776,19 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C3" s="2">
-        <v>21</v>
+        <v>291</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="2">
-        <v>232</v>
+        <v>293</v>
       </c>
       <c r="F3" s="2">
-        <v>24</v>
+        <v>294</v>
       </c>
       <c r="G3" s="2">
-        <v>25</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.5">
@@ -799,19 +799,19 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="C4" s="2">
-        <v>21</v>
+        <v>201</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
       <c r="E4" s="2">
-        <v>23</v>
+        <v>203</v>
       </c>
       <c r="F4" s="2">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="G4" s="2">
-        <v>25</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.5">
@@ -822,19 +822,19 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="2">
-        <v>21</v>
+        <v>211</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <v>23</v>
+        <v>213</v>
       </c>
       <c r="F5" s="2">
-        <v>24</v>
+        <v>214</v>
       </c>
       <c r="G5" s="2">
-        <v>252</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.5">
@@ -845,19 +845,19 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C6" s="2">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>23</v>
+        <v>223</v>
       </c>
       <c r="F6" s="2">
-        <v>24</v>
+        <v>224</v>
       </c>
       <c r="G6" s="2">
-        <v>25</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.5">
@@ -868,19 +868,19 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C7" s="2">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F7" s="2">
-        <v>24</v>
+        <v>234</v>
       </c>
       <c r="G7" s="2">
-        <v>25</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.5">
@@ -891,19 +891,19 @@
         <v>0.625</v>
       </c>
       <c r="C8" s="2">
-        <v>131</v>
+        <v>241</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>60</v>
+        <v>243</v>
       </c>
       <c r="F8" s="2">
-        <v>131</v>
+        <v>244</v>
       </c>
       <c r="G8" s="2">
-        <v>60</v>
+        <v>245</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -915,19 +915,19 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="C9" s="2">
-        <v>13</v>
+        <v>251</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <v>12</v>
+        <v>253</v>
       </c>
       <c r="F9" s="2">
-        <v>13</v>
+        <v>254</v>
       </c>
       <c r="G9" s="2">
-        <v>12</v>
+        <v>255</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -939,19 +939,19 @@
         <v>0.70833333333333404</v>
       </c>
       <c r="C10" s="2">
-        <v>131</v>
+        <v>261</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <v>121</v>
+        <v>263</v>
       </c>
       <c r="F10" s="2">
-        <v>131</v>
+        <v>264</v>
       </c>
       <c r="G10" s="2">
-        <v>121</v>
+        <v>265</v>
       </c>
       <c r="H10" s="2"/>
     </row>
@@ -963,19 +963,19 @@
         <v>0.750000000000001</v>
       </c>
       <c r="C11" s="2">
-        <v>13</v>
+        <v>271</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>121</v>
+        <v>273</v>
       </c>
       <c r="F11" s="2">
-        <v>13</v>
+        <v>274</v>
       </c>
       <c r="G11" s="2">
-        <v>121</v>
+        <v>275</v>
       </c>
       <c r="H11" s="2"/>
     </row>
@@ -989,7 +989,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C2" sqref="C2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1028,19 +1028,19 @@
         <v>0.38194444444444442</v>
       </c>
       <c r="C2">
-        <v>313</v>
+        <v>381</v>
       </c>
       <c r="D2">
-        <v>32</v>
+        <v>382</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>34</v>
-      </c>
-      <c r="G2">
-        <v>35</v>
+      <c r="F2" s="2">
+        <v>384</v>
+      </c>
+      <c r="G2" s="2">
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.5">
@@ -1051,19 +1051,19 @@
         <v>0.4236111111111111</v>
       </c>
       <c r="C3">
-        <v>31</v>
+        <v>391</v>
       </c>
       <c r="D3">
-        <v>32</v>
+        <v>392</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>343</v>
-      </c>
-      <c r="G3">
-        <v>35</v>
+      <c r="F3" s="2">
+        <v>394</v>
+      </c>
+      <c r="G3" s="2">
+        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
@@ -1074,19 +1074,19 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="C4">
-        <v>31</v>
+        <v>301</v>
       </c>
       <c r="D4">
-        <v>323</v>
+        <v>302</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>34</v>
-      </c>
-      <c r="G4">
-        <v>35</v>
+      <c r="F4" s="2">
+        <v>304</v>
+      </c>
+      <c r="G4" s="2">
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
@@ -1097,19 +1097,19 @@
         <v>0.5</v>
       </c>
       <c r="C5">
-        <v>31</v>
+        <v>311</v>
       </c>
       <c r="D5">
-        <v>32</v>
+        <v>312</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
-        <v>34</v>
-      </c>
-      <c r="G5">
-        <v>353</v>
+      <c r="F5" s="2">
+        <v>314</v>
+      </c>
+      <c r="G5" s="2">
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
@@ -1120,19 +1120,19 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="C6">
-        <v>31</v>
+        <v>321</v>
       </c>
       <c r="D6">
-        <v>32</v>
+        <v>322</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>34</v>
-      </c>
-      <c r="G6">
-        <v>35</v>
+      <c r="F6" s="2">
+        <v>324</v>
+      </c>
+      <c r="G6" s="2">
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
@@ -1143,19 +1143,19 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="C7">
-        <v>31</v>
+        <v>331</v>
       </c>
       <c r="D7">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>34</v>
-      </c>
-      <c r="G7">
-        <v>353</v>
+      <c r="F7" s="2">
+        <v>334</v>
+      </c>
+      <c r="G7" s="2">
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.5">
@@ -1165,20 +1165,20 @@
       <c r="B8" s="1">
         <v>0.624999999999999</v>
       </c>
-      <c r="C8" s="2">
-        <v>60</v>
-      </c>
-      <c r="D8" s="2">
-        <v>131</v>
+      <c r="C8">
+        <v>341</v>
+      </c>
+      <c r="D8">
+        <v>342</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>60</v>
+        <v>344</v>
       </c>
       <c r="G8" s="2">
-        <v>131</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.5">
@@ -1188,20 +1188,20 @@
       <c r="B9" s="1">
         <v>0.66666666666666496</v>
       </c>
-      <c r="C9" s="2">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2">
-        <v>13</v>
+      <c r="C9">
+        <v>351</v>
+      </c>
+      <c r="D9">
+        <v>352</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>12</v>
+        <v>354</v>
       </c>
       <c r="G9" s="2">
-        <v>13</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.5">
@@ -1211,20 +1211,20 @@
       <c r="B10" s="1">
         <v>0.70833333333333104</v>
       </c>
-      <c r="C10" s="2">
-        <v>121</v>
-      </c>
-      <c r="D10" s="2">
-        <v>131</v>
+      <c r="C10">
+        <v>361</v>
+      </c>
+      <c r="D10">
+        <v>362</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>121</v>
+        <v>364</v>
       </c>
       <c r="G10" s="2">
-        <v>131</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
@@ -1234,20 +1234,20 @@
       <c r="B11" s="1">
         <v>0.749999999999997</v>
       </c>
-      <c r="C11" s="2">
-        <v>121</v>
-      </c>
-      <c r="D11" s="2">
-        <v>13</v>
+      <c r="C11">
+        <v>371</v>
+      </c>
+      <c r="D11">
+        <v>372</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" s="2">
-        <v>121</v>
+        <v>374</v>
       </c>
       <c r="G11" s="2">
-        <v>13</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -1260,7 +1260,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C2" sqref="C2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1299,19 +1299,19 @@
         <v>0.3756944444444445</v>
       </c>
       <c r="C2">
-        <v>414</v>
+        <v>481</v>
       </c>
       <c r="D2">
-        <v>42</v>
+        <v>482</v>
       </c>
       <c r="E2">
-        <v>434</v>
+        <v>483</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>45</v>
+        <v>485</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.5">
@@ -1322,19 +1322,19 @@
         <v>0.41736111111111113</v>
       </c>
       <c r="C3">
-        <v>41</v>
+        <v>491</v>
       </c>
       <c r="D3">
-        <v>424</v>
+        <v>492</v>
       </c>
       <c r="E3">
-        <v>43</v>
+        <v>493</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>454</v>
+        <v>495</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.5">
@@ -1345,19 +1345,19 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="C4">
-        <v>41</v>
+        <v>401</v>
       </c>
       <c r="D4">
-        <v>42</v>
+        <v>402</v>
       </c>
       <c r="E4">
-        <v>43</v>
+        <v>403</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>45</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.5">
@@ -1368,19 +1368,19 @@
         <v>0.5</v>
       </c>
       <c r="C5">
-        <v>41</v>
+        <v>411</v>
       </c>
       <c r="D5">
-        <v>42</v>
+        <v>412</v>
       </c>
       <c r="E5">
-        <v>434</v>
+        <v>413</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>45</v>
+        <v>415</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.5">
@@ -1391,19 +1391,19 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="C6">
-        <v>41</v>
+        <v>421</v>
       </c>
       <c r="D6">
-        <v>42</v>
+        <v>422</v>
       </c>
       <c r="E6">
-        <v>43</v>
+        <v>423</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>454</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.5">
@@ -1414,19 +1414,19 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="C7">
-        <v>41</v>
+        <v>431</v>
       </c>
       <c r="D7">
-        <v>424</v>
+        <v>432</v>
       </c>
       <c r="E7">
-        <v>43</v>
+        <v>433</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>45</v>
+        <v>435</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.5">
@@ -1436,20 +1436,20 @@
       <c r="B8" s="1">
         <v>0.624999999999999</v>
       </c>
-      <c r="C8" s="2">
-        <v>60</v>
-      </c>
-      <c r="D8" s="2">
-        <v>131</v>
-      </c>
-      <c r="E8" s="2">
-        <v>60</v>
+      <c r="C8">
+        <v>441</v>
+      </c>
+      <c r="D8">
+        <v>442</v>
+      </c>
+      <c r="E8">
+        <v>443</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="2">
-        <v>60</v>
+      <c r="G8">
+        <v>445</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -1460,20 +1460,20 @@
       <c r="B9" s="1">
         <v>0.66666666666666496</v>
       </c>
-      <c r="C9" s="2">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2">
-        <v>12</v>
+      <c r="C9">
+        <v>451</v>
+      </c>
+      <c r="D9">
+        <v>452</v>
+      </c>
+      <c r="E9">
+        <v>453</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" s="2">
-        <v>12</v>
+      <c r="G9">
+        <v>455</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -1484,20 +1484,20 @@
       <c r="B10" s="1">
         <v>0.70833333333333104</v>
       </c>
-      <c r="C10" s="2">
-        <v>121</v>
-      </c>
-      <c r="D10" s="2">
-        <v>131</v>
-      </c>
-      <c r="E10" s="2">
-        <v>121</v>
+      <c r="C10">
+        <v>461</v>
+      </c>
+      <c r="D10">
+        <v>462</v>
+      </c>
+      <c r="E10">
+        <v>463</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="G10" s="2">
-        <v>121</v>
+      <c r="G10">
+        <v>465</v>
       </c>
       <c r="H10" s="2"/>
     </row>
@@ -1508,20 +1508,20 @@
       <c r="B11" s="1">
         <v>0.749999999999997</v>
       </c>
-      <c r="C11" s="2">
-        <v>121</v>
-      </c>
-      <c r="D11" s="2">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2">
-        <v>121</v>
+      <c r="C11">
+        <v>471</v>
+      </c>
+      <c r="D11">
+        <v>472</v>
+      </c>
+      <c r="E11">
+        <v>473</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11" s="2">
-        <v>121</v>
+      <c r="G11">
+        <v>475</v>
       </c>
       <c r="H11" s="2"/>
     </row>
@@ -1535,7 +1535,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1574,16 +1574,16 @@
         <v>0.375</v>
       </c>
       <c r="C2">
-        <v>51</v>
+        <v>581</v>
       </c>
       <c r="D2">
-        <v>525</v>
+        <v>582</v>
       </c>
       <c r="E2">
-        <v>53</v>
+        <v>583</v>
       </c>
       <c r="F2">
-        <v>54</v>
+        <v>584</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1597,16 +1597,16 @@
         <v>0.41736111111111113</v>
       </c>
       <c r="C3">
-        <v>51</v>
+        <v>591</v>
       </c>
       <c r="D3">
-        <v>525</v>
+        <v>592</v>
       </c>
       <c r="E3">
-        <v>53</v>
+        <v>593</v>
       </c>
       <c r="F3">
-        <v>54</v>
+        <v>594</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1620,16 +1620,16 @@
         <v>0.45902777777777781</v>
       </c>
       <c r="C4">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="D4">
-        <v>52</v>
+        <v>502</v>
       </c>
       <c r="E4">
-        <v>53</v>
+        <v>503</v>
       </c>
       <c r="F4">
-        <v>54</v>
+        <v>504</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1643,16 +1643,16 @@
         <v>0.5</v>
       </c>
       <c r="C5">
-        <v>51</v>
+        <v>511</v>
       </c>
       <c r="D5">
-        <v>52</v>
+        <v>512</v>
       </c>
       <c r="E5">
-        <v>53</v>
+        <v>513</v>
       </c>
       <c r="F5">
-        <v>545</v>
+        <v>514</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1666,16 +1666,16 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C6">
-        <v>51</v>
+        <v>521</v>
       </c>
       <c r="D6">
-        <v>52</v>
+        <v>522</v>
       </c>
       <c r="E6">
-        <v>535</v>
+        <v>523</v>
       </c>
       <c r="F6">
-        <v>54</v>
+        <v>524</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1689,16 +1689,16 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C7">
-        <v>51</v>
+        <v>531</v>
       </c>
       <c r="D7">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="E7">
-        <v>53</v>
+        <v>533</v>
       </c>
       <c r="F7">
-        <v>54</v>
+        <v>534</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1711,17 +1711,17 @@
       <c r="B8" s="3">
         <v>0.625</v>
       </c>
-      <c r="C8" s="2">
-        <v>60</v>
-      </c>
-      <c r="D8" s="2">
-        <v>131</v>
-      </c>
-      <c r="E8" s="2">
-        <v>60</v>
-      </c>
-      <c r="F8" s="2">
-        <v>50</v>
+      <c r="C8">
+        <v>541</v>
+      </c>
+      <c r="D8">
+        <v>542</v>
+      </c>
+      <c r="E8">
+        <v>543</v>
+      </c>
+      <c r="F8">
+        <v>544</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1734,17 +1734,17 @@
       <c r="B9" s="3">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C9" s="2">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2">
-        <v>12</v>
-      </c>
-      <c r="F9" s="2">
-        <v>200</v>
+      <c r="C9">
+        <v>551</v>
+      </c>
+      <c r="D9">
+        <v>552</v>
+      </c>
+      <c r="E9">
+        <v>553</v>
+      </c>
+      <c r="F9">
+        <v>554</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1757,17 +1757,17 @@
       <c r="B10" s="3">
         <v>0.70833333333333404</v>
       </c>
-      <c r="C10" s="2">
-        <v>121</v>
-      </c>
-      <c r="D10" s="2">
-        <v>131</v>
-      </c>
-      <c r="E10" s="2">
-        <v>121</v>
-      </c>
-      <c r="F10" s="2">
-        <v>300</v>
+      <c r="C10">
+        <v>561</v>
+      </c>
+      <c r="D10">
+        <v>562</v>
+      </c>
+      <c r="E10">
+        <v>563</v>
+      </c>
+      <c r="F10">
+        <v>564</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1780,17 +1780,17 @@
       <c r="B11" s="3">
         <v>0.750000000000001</v>
       </c>
-      <c r="C11" s="2">
-        <v>121</v>
-      </c>
-      <c r="D11" s="2">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2">
-        <v>121</v>
-      </c>
-      <c r="F11" s="2">
-        <v>50</v>
+      <c r="C11">
+        <v>571</v>
+      </c>
+      <c r="D11">
+        <v>572</v>
+      </c>
+      <c r="E11">
+        <v>573</v>
+      </c>
+      <c r="F11">
+        <v>574</v>
       </c>
       <c r="G11">
         <v>0</v>

</xml_diff>

<commit_message>
start develop inbound mode
</commit_message>
<xml_diff>
--- a/Service_plan_form/demand_format/demandTFtestXLSX_new.xlsx
+++ b/Service_plan_form/demand_format/demandTFtestXLSX_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATCHAPCYP\Repository\Service_plan_form\Service_plan_form\demand_format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ite004\Repository\service_plan_form\Service_plan_form\demand_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B094F2-700A-4A30-BE54-07B098FF502A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F1327D-1B4D-4613-A19C-3726CDD7BF4C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4372" yWindow="923" windowWidth="14400" windowHeight="8272" activeTab="4" xr2:uid="{D39FB900-15C1-7B47-8F01-B0CA86C94EDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D39FB900-15C1-7B47-8F01-B0CA86C94EDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Station1" sheetId="1" r:id="rId1"/>
@@ -57,20 +57,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="187" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -97,9 +97,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="187" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,16 +437,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783E6E19-8982-3D4E-8148-6314C244FA37}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -469,7 +469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0.33333333333333331</v>
       </c>
@@ -480,19 +480,19 @@
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>182</v>
+        <v>882</v>
       </c>
       <c r="E2" s="2">
-        <v>183</v>
+        <v>500</v>
       </c>
       <c r="F2" s="2">
-        <v>184</v>
+        <v>284</v>
       </c>
       <c r="G2" s="2">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>0.375</v>
       </c>
@@ -503,19 +503,19 @@
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>192</v>
+        <v>692</v>
       </c>
       <c r="E3" s="2">
         <v>193</v>
       </c>
       <c r="F3" s="2">
-        <v>194</v>
+        <v>294</v>
       </c>
       <c r="G3" s="2">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>0.41666666666666669</v>
       </c>
@@ -538,7 +538,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>0.45833333333333331</v>
       </c>
@@ -552,16 +552,16 @@
         <v>112</v>
       </c>
       <c r="E5" s="2">
-        <v>113</v>
+        <v>313</v>
       </c>
       <c r="F5" s="2">
         <v>114</v>
       </c>
       <c r="G5" s="2">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>0.5</v>
       </c>
@@ -572,19 +572,19 @@
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>122</v>
+        <v>322</v>
       </c>
       <c r="E6" s="2">
         <v>123</v>
       </c>
       <c r="F6" s="2">
-        <v>124</v>
+        <v>324</v>
       </c>
       <c r="G6" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>0.54166666666666663</v>
       </c>
@@ -607,7 +607,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>0.58333333333333304</v>
       </c>
@@ -618,19 +618,19 @@
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>142</v>
+        <v>242</v>
       </c>
       <c r="E8" s="2">
         <v>143</v>
       </c>
       <c r="F8" s="2">
-        <v>144</v>
+        <v>244</v>
       </c>
       <c r="G8" s="2">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>0.625</v>
       </c>
@@ -653,7 +653,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>0.66666666666666696</v>
       </c>
@@ -664,19 +664,19 @@
         <v>0</v>
       </c>
       <c r="D10" s="2">
-        <v>162</v>
+        <v>882</v>
       </c>
       <c r="E10" s="2">
-        <v>163</v>
+        <v>500</v>
       </c>
       <c r="F10" s="2">
-        <v>164</v>
+        <v>284</v>
       </c>
       <c r="G10" s="2">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>0.70833333333333304</v>
       </c>
@@ -687,16 +687,16 @@
         <v>0</v>
       </c>
       <c r="D11" s="2">
-        <v>172</v>
+        <v>692</v>
       </c>
       <c r="E11" s="2">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="F11" s="2">
-        <v>174</v>
+        <v>294</v>
       </c>
       <c r="G11" s="2">
-        <v>175</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -714,15 +714,15 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -745,7 +745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0.33333333333333331</v>
       </c>
@@ -768,7 +768,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>0.375</v>
       </c>
@@ -791,7 +791,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>0.41666666666666669</v>
       </c>
@@ -805,7 +805,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2">
-        <v>203</v>
+        <v>340</v>
       </c>
       <c r="F4" s="2">
         <v>204</v>
@@ -814,7 +814,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>0.45833333333333331</v>
       </c>
@@ -831,13 +831,13 @@
         <v>213</v>
       </c>
       <c r="F5" s="2">
-        <v>214</v>
+        <v>414</v>
       </c>
       <c r="G5" s="2">
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>0.5</v>
       </c>
@@ -860,7 +860,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>0.54166666666666663</v>
       </c>
@@ -880,10 +880,10 @@
         <v>234</v>
       </c>
       <c r="G7" s="2">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>0.58333333333333304</v>
       </c>
@@ -897,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>243</v>
+        <v>143</v>
       </c>
       <c r="F8" s="2">
         <v>244</v>
@@ -907,7 +907,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>0.625</v>
       </c>
@@ -931,7 +931,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>0.66666666666666696</v>
       </c>
@@ -948,14 +948,14 @@
         <v>263</v>
       </c>
       <c r="F10" s="2">
-        <v>264</v>
+        <v>664</v>
       </c>
       <c r="G10" s="2">
         <v>265</v>
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>0.70833333333333304</v>
       </c>
@@ -969,13 +969,13 @@
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>273</v>
+        <v>173</v>
       </c>
       <c r="F11" s="2">
         <v>274</v>
       </c>
       <c r="G11" s="2">
-        <v>275</v>
+        <v>475</v>
       </c>
       <c r="H11" s="2"/>
     </row>
@@ -989,15 +989,15 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D11"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0.33333333333333331</v>
       </c>
@@ -1037,13 +1037,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>384</v>
+        <v>284</v>
       </c>
       <c r="G2" s="2">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.375</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0.41666666666666702</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>301</v>
       </c>
       <c r="D4">
-        <v>302</v>
+        <v>202</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1089,7 +1089,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.45833333333333298</v>
       </c>
@@ -1106,13 +1106,13 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>314</v>
+        <v>114</v>
       </c>
       <c r="G5" s="2">
         <v>315</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.5</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="C6">
-        <v>321</v>
+        <v>221</v>
       </c>
       <c r="D6">
         <v>322</v>
@@ -1132,10 +1132,10 @@
         <v>324</v>
       </c>
       <c r="G6" s="2">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0.54166666666666696</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0.58333333333333404</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>341</v>
       </c>
       <c r="D8">
-        <v>342</v>
+        <v>142</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1178,10 +1178,10 @@
         <v>344</v>
       </c>
       <c r="G8" s="2">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0.625000000000001</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>0.66666666666666496</v>
       </c>
       <c r="C9">
-        <v>351</v>
+        <v>151</v>
       </c>
       <c r="D9">
         <v>352</v>
@@ -1201,10 +1201,10 @@
         <v>354</v>
       </c>
       <c r="G9" s="2">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0.66666666666666796</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>361</v>
       </c>
       <c r="D10">
-        <v>362</v>
+        <v>162</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1224,10 +1224,10 @@
         <v>364</v>
       </c>
       <c r="G10" s="2">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0.70833333333333504</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>0.749999999999997</v>
       </c>
       <c r="C11">
-        <v>371</v>
+        <v>171</v>
       </c>
       <c r="D11">
         <v>372</v>
@@ -1244,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2">
-        <v>374</v>
+        <v>174</v>
       </c>
       <c r="G11" s="2">
         <v>375</v>
@@ -1260,15 +1260,15 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E11"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0.33333333333333331</v>
       </c>
@@ -1311,10 +1311,10 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.375</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0.41666666666666702</v>
       </c>
@@ -1357,10 +1357,10 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.45833333333333298</v>
       </c>
@@ -1380,10 +1380,10 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.5</v>
       </c>
@@ -1403,10 +1403,10 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0.54166666666666696</v>
       </c>
@@ -1426,10 +1426,10 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0.58333333333333404</v>
       </c>
@@ -1449,11 +1449,11 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>445</v>
+        <v>100</v>
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0.625000000000001</v>
       </c>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0.66666666666666796</v>
       </c>
@@ -1497,11 +1497,11 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>465</v>
+        <v>365</v>
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0.70833333333333504</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>475</v>
+        <v>175</v>
       </c>
       <c r="H11" s="2"/>
     </row>
@@ -1534,16 +1534,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1338C68A-BFB5-4B6E-84B8-51079048C625}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0.33333333333333331</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>0.375</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>0.41666666666666669</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>0.45833333333333331</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>0.5</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>0.54166666666666663</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>0.58333333333333304</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>0.625</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>0.66666666666666696</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>0.70833333333333304</v>
       </c>

</xml_diff>

<commit_message>
fix before present proj
</commit_message>
<xml_diff>
--- a/Service_plan_form/demand_format/demandTFtestXLSX_new.xlsx
+++ b/Service_plan_form/demand_format/demandTFtestXLSX_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atchapcyp\Repository\Privateworkspace\service_plan_form\service_plan_form\Service_plan_form\demand_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06967369-B7A1-4723-A2B3-69BCDC515998}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AEA5EB-1D24-411D-B733-255362CBD65D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{D39FB900-15C1-7B47-8F01-B0CA86C94EDD}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:G11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -474,7 +474,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="3">
-        <v>0.3756944444444445</v>
+        <v>0.375</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -714,7 +714,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -750,7 +750,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="3">
-        <v>0.3756944444444445</v>
+        <v>0.375</v>
       </c>
       <c r="C2" s="2">
         <v>281</v>
@@ -989,7 +989,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1025,7 +1025,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="1">
-        <v>0.38194444444444442</v>
+        <v>0.375</v>
       </c>
       <c r="C2">
         <v>381</v>
@@ -1048,7 +1048,7 @@
         <v>0.375</v>
       </c>
       <c r="B3" s="1">
-        <v>0.4236111111111111</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C3">
         <v>391</v>
@@ -1260,7 +1260,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1296,7 +1296,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="1">
-        <v>0.3756944444444445</v>
+        <v>0.375</v>
       </c>
       <c r="C2">
         <v>81</v>
@@ -1319,7 +1319,7 @@
         <v>0.375</v>
       </c>
       <c r="B3" s="1">
-        <v>0.41736111111111113</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C3">
         <v>61</v>
@@ -1535,7 +1535,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1594,7 @@
         <v>0.375</v>
       </c>
       <c r="B3" s="3">
-        <v>0.41736111111111113</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C3" s="2">
         <v>692</v>
@@ -1617,7 +1617,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B4" s="3">
-        <v>0.45902777777777781</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="C4" s="2">
         <v>102</v>

</xml_diff>